<commit_message>
before start every n day
</commit_message>
<xml_diff>
--- a/Account_starts_by_DD_and_profit/profit_trigger_optimization_results.xlsx
+++ b/Account_starts_by_DD_and_profit/profit_trigger_optimization_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,22 +500,22 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="E2" t="n">
-        <v>2346230</v>
+        <v>348499</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="G2" t="n">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="H2" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="I2" t="n">
-        <v>-164084</v>
+        <v>-24206</v>
       </c>
     </row>
     <row r="3">
@@ -527,22 +527,22 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>200</v>
+        <v>3100</v>
       </c>
       <c r="E3" t="n">
-        <v>2107417</v>
+        <v>341900</v>
       </c>
       <c r="F3" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="G3" t="n">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="H3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="I3" t="n">
-        <v>-177934</v>
+        <v>-25177</v>
       </c>
     </row>
     <row r="4">
@@ -554,22 +554,22 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>300</v>
+        <v>3200</v>
       </c>
       <c r="E4" t="n">
-        <v>1774179</v>
+        <v>325976</v>
       </c>
       <c r="F4" t="n">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="G4" t="n">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H4" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="I4" t="n">
-        <v>-143343</v>
+        <v>-23506</v>
       </c>
     </row>
     <row r="5">
@@ -581,22 +581,22 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>400</v>
+        <v>3300</v>
       </c>
       <c r="E5" t="n">
-        <v>1423526</v>
+        <v>297727</v>
       </c>
       <c r="F5" t="n">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="G5" t="n">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="H5" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="I5" t="n">
-        <v>-108780</v>
+        <v>-22314</v>
       </c>
     </row>
     <row r="6">
@@ -608,22 +608,22 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>500</v>
+        <v>3400</v>
       </c>
       <c r="E6" t="n">
-        <v>1381126</v>
+        <v>293229</v>
       </c>
       <c r="F6" t="n">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="G6" t="n">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="H6" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="I6" t="n">
-        <v>-103094</v>
+        <v>-21676</v>
       </c>
     </row>
     <row r="7">
@@ -635,22 +635,22 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>600</v>
+        <v>3500</v>
       </c>
       <c r="E7" t="n">
-        <v>1155978</v>
+        <v>283844</v>
       </c>
       <c r="F7" t="n">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="G7" t="n">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H7" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>-89590</v>
+        <v>-20141</v>
       </c>
     </row>
     <row r="8">
@@ -662,22 +662,22 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>700</v>
+        <v>3800</v>
       </c>
       <c r="E8" t="n">
-        <v>1036673</v>
+        <v>282968</v>
       </c>
       <c r="F8" t="n">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="G8" t="n">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="H8" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="I8" t="n">
-        <v>-77513</v>
+        <v>-20484</v>
       </c>
     </row>
     <row r="9">
@@ -689,22 +689,22 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
-        <v>800</v>
+        <v>3600</v>
       </c>
       <c r="E9" t="n">
-        <v>910778</v>
+        <v>282471</v>
       </c>
       <c r="F9" t="n">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="G9" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="H9" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
-        <v>-69636</v>
+        <v>-21515</v>
       </c>
     </row>
     <row r="10">
@@ -716,22 +716,22 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>900</v>
+        <v>3700</v>
       </c>
       <c r="E10" t="n">
-        <v>871562</v>
+        <v>276465</v>
       </c>
       <c r="F10" t="n">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="G10" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="H10" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="I10" t="n">
-        <v>-65324</v>
+        <v>-20484</v>
       </c>
     </row>
     <row r="11">
@@ -743,22 +743,22 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
-        <v>1000</v>
+        <v>3900</v>
       </c>
       <c r="E11" t="n">
-        <v>857654</v>
+        <v>271853</v>
       </c>
       <c r="F11" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G11" t="n">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="H11" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>-63703</v>
+        <v>-19367</v>
       </c>
     </row>
     <row r="12">
@@ -770,22 +770,22 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
-        <v>1100</v>
+        <v>4000</v>
       </c>
       <c r="E12" t="n">
-        <v>711235</v>
+        <v>270650</v>
       </c>
       <c r="F12" t="n">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="G12" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="H12" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="I12" t="n">
-        <v>-53024</v>
+        <v>-19367</v>
       </c>
     </row>
     <row r="13">
@@ -797,22 +797,22 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
-        <v>1300</v>
+        <v>4100</v>
       </c>
       <c r="E13" t="n">
-        <v>691329</v>
+        <v>266058</v>
       </c>
       <c r="F13" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G13" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="H13" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I13" t="n">
-        <v>-50864</v>
+        <v>-19018</v>
       </c>
     </row>
     <row r="14">
@@ -824,22 +824,22 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
-        <v>1200</v>
+        <v>4200</v>
       </c>
       <c r="E14" t="n">
-        <v>683540</v>
+        <v>256386</v>
       </c>
       <c r="F14" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="G14" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H14" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I14" t="n">
-        <v>-50226</v>
+        <v>-18652</v>
       </c>
     </row>
     <row r="15">
@@ -851,22 +851,22 @@
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
-        <v>1400</v>
+        <v>4300</v>
       </c>
       <c r="E15" t="n">
-        <v>659133</v>
+        <v>252426</v>
       </c>
       <c r="F15" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G15" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="H15" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I15" t="n">
-        <v>-48817</v>
+        <v>-18147</v>
       </c>
     </row>
     <row r="16">
@@ -878,22 +878,22 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
-        <v>1500</v>
+        <v>4400</v>
       </c>
       <c r="E16" t="n">
-        <v>629888</v>
+        <v>247923</v>
       </c>
       <c r="F16" t="n">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="G16" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="H16" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I16" t="n">
-        <v>-45116</v>
+        <v>-16891</v>
       </c>
     </row>
     <row r="17">
@@ -905,22 +905,22 @@
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
-        <v>1600</v>
+        <v>4500</v>
       </c>
       <c r="E17" t="n">
-        <v>602148</v>
+        <v>245722</v>
       </c>
       <c r="F17" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="G17" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H17" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I17" t="n">
-        <v>-43156</v>
+        <v>-17367</v>
       </c>
     </row>
     <row r="18">
@@ -932,22 +932,22 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
-        <v>1700</v>
+        <v>4700</v>
       </c>
       <c r="E18" t="n">
-        <v>502848</v>
+        <v>234645</v>
       </c>
       <c r="F18" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="G18" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="H18" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I18" t="n">
-        <v>-38427</v>
+        <v>-17853</v>
       </c>
     </row>
     <row r="19">
@@ -959,22 +959,22 @@
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>1900</v>
+        <v>4600</v>
       </c>
       <c r="E19" t="n">
-        <v>483978</v>
+        <v>232216</v>
       </c>
       <c r="F19" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="G19" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="H19" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I19" t="n">
-        <v>-35578</v>
+        <v>-17853</v>
       </c>
     </row>
     <row r="20">
@@ -986,22 +986,22 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
-        <v>2000</v>
+        <v>4800</v>
       </c>
       <c r="E20" t="n">
-        <v>476106</v>
+        <v>229074</v>
       </c>
       <c r="F20" t="n">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="G20" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H20" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I20" t="n">
-        <v>-34626</v>
+        <v>-16822</v>
       </c>
     </row>
     <row r="21">
@@ -1013,22 +1013,22 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
-        <v>1800</v>
+        <v>4900</v>
       </c>
       <c r="E21" t="n">
-        <v>472258</v>
+        <v>222044</v>
       </c>
       <c r="F21" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G21" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="H21" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
-        <v>-35953</v>
+        <v>-14648</v>
       </c>
     </row>
     <row r="22">
@@ -1040,265 +1040,22 @@
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
-        <v>2100</v>
+        <v>5000</v>
       </c>
       <c r="E22" t="n">
-        <v>469420</v>
+        <v>219821</v>
       </c>
       <c r="F22" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G22" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H22" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>-34332</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="b">
-        <v>0</v>
-      </c>
-      <c r="B23" t="b">
-        <v>1</v>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="n">
-        <v>2200</v>
-      </c>
-      <c r="E23" t="n">
-        <v>450648</v>
-      </c>
-      <c r="F23" t="n">
-        <v>26</v>
-      </c>
-      <c r="G23" t="n">
-        <v>19</v>
-      </c>
-      <c r="H23" t="n">
-        <v>7</v>
-      </c>
-      <c r="I23" t="n">
-        <v>-32795</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="b">
-        <v>0</v>
-      </c>
-      <c r="B24" t="b">
-        <v>1</v>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="n">
-        <v>2300</v>
-      </c>
-      <c r="E24" t="n">
-        <v>436154</v>
-      </c>
-      <c r="F24" t="n">
-        <v>24</v>
-      </c>
-      <c r="G24" t="n">
-        <v>18</v>
-      </c>
-      <c r="H24" t="n">
-        <v>6</v>
-      </c>
-      <c r="I24" t="n">
-        <v>-31916</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="b">
-        <v>0</v>
-      </c>
-      <c r="B25" t="b">
-        <v>1</v>
-      </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="n">
-        <v>2500</v>
-      </c>
-      <c r="E25" t="n">
-        <v>410238</v>
-      </c>
-      <c r="F25" t="n">
-        <v>24</v>
-      </c>
-      <c r="G25" t="n">
-        <v>17</v>
-      </c>
-      <c r="H25" t="n">
-        <v>7</v>
-      </c>
-      <c r="I25" t="n">
-        <v>-29638</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="b">
-        <v>0</v>
-      </c>
-      <c r="B26" t="b">
-        <v>1</v>
-      </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="n">
-        <v>2600</v>
-      </c>
-      <c r="E26" t="n">
-        <v>393377</v>
-      </c>
-      <c r="F26" t="n">
-        <v>23</v>
-      </c>
-      <c r="G26" t="n">
-        <v>16</v>
-      </c>
-      <c r="H26" t="n">
-        <v>7</v>
-      </c>
-      <c r="I26" t="n">
-        <v>-28839</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="b">
-        <v>0</v>
-      </c>
-      <c r="B27" t="b">
-        <v>1</v>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="n">
-        <v>2400</v>
-      </c>
-      <c r="E27" t="n">
-        <v>390644</v>
-      </c>
-      <c r="F27" t="n">
-        <v>23</v>
-      </c>
-      <c r="G27" t="n">
-        <v>17</v>
-      </c>
-      <c r="H27" t="n">
-        <v>6</v>
-      </c>
-      <c r="I27" t="n">
-        <v>-29638</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B28" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="n">
-        <v>2700</v>
-      </c>
-      <c r="E28" t="n">
-        <v>384596</v>
-      </c>
-      <c r="F28" t="n">
-        <v>21</v>
-      </c>
-      <c r="G28" t="n">
-        <v>16</v>
-      </c>
-      <c r="H28" t="n">
-        <v>5</v>
-      </c>
-      <c r="I28" t="n">
-        <v>-27808</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="b">
-        <v>0</v>
-      </c>
-      <c r="B29" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="n">
-        <v>2800</v>
-      </c>
-      <c r="E29" t="n">
-        <v>373242</v>
-      </c>
-      <c r="F29" t="n">
-        <v>20</v>
-      </c>
-      <c r="G29" t="n">
-        <v>16</v>
-      </c>
-      <c r="H29" t="n">
-        <v>4</v>
-      </c>
-      <c r="I29" t="n">
-        <v>-26257</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="b">
-        <v>0</v>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="n">
-        <v>2900</v>
-      </c>
-      <c r="E30" t="n">
-        <v>362358</v>
-      </c>
-      <c r="F30" t="n">
-        <v>20</v>
-      </c>
-      <c r="G30" t="n">
-        <v>15</v>
-      </c>
-      <c r="H30" t="n">
-        <v>5</v>
-      </c>
-      <c r="I30" t="n">
-        <v>-26423</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="b">
-        <v>0</v>
-      </c>
-      <c r="B31" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E31" t="n">
-        <v>348499</v>
-      </c>
-      <c r="F31" t="n">
-        <v>19</v>
-      </c>
-      <c r="G31" t="n">
-        <v>15</v>
-      </c>
-      <c r="H31" t="n">
-        <v>4</v>
-      </c>
-      <c r="I31" t="n">
-        <v>-24206</v>
+        <v>-14648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
waiting for recovery only for DD starts
</commit_message>
<xml_diff>
--- a/Account_starts_by_DD_and_profit/profit_trigger_optimization_results.xlsx
+++ b/Account_starts_by_DD_and_profit/profit_trigger_optimization_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,22 +516,22 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="G2" t="n">
-        <v>88776</v>
+        <v>237634</v>
       </c>
       <c r="H2" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I2" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>-6441</v>
+        <v>-17823</v>
       </c>
     </row>
     <row r="3">
@@ -547,22 +547,22 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>3100</v>
+        <v>1100</v>
       </c>
       <c r="G3" t="n">
-        <v>86796</v>
+        <v>221181</v>
       </c>
       <c r="H3" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I3" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-6441</v>
+        <v>-17176</v>
       </c>
     </row>
     <row r="4">
@@ -578,22 +578,22 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>3200</v>
+        <v>1200</v>
       </c>
       <c r="G4" t="n">
-        <v>84652</v>
+        <v>205660</v>
       </c>
       <c r="H4" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I4" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>-6441</v>
+        <v>-16102</v>
       </c>
     </row>
     <row r="5">
@@ -609,22 +609,22 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>3300</v>
+        <v>1300</v>
       </c>
       <c r="G5" t="n">
-        <v>84538</v>
+        <v>195813</v>
       </c>
       <c r="H5" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I5" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>-6441</v>
+        <v>-15029</v>
       </c>
     </row>
     <row r="6">
@@ -640,22 +640,22 @@
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>3400</v>
+        <v>1400</v>
       </c>
       <c r="G6" t="n">
-        <v>80956</v>
+        <v>180994</v>
       </c>
       <c r="H6" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="I6" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>-6441</v>
+        <v>-13956</v>
       </c>
     </row>
     <row r="7">
@@ -671,22 +671,22 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>3500</v>
+        <v>1500</v>
       </c>
       <c r="G7" t="n">
-        <v>79974</v>
+        <v>165537</v>
       </c>
       <c r="H7" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I7" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>-6441</v>
+        <v>-12882</v>
       </c>
     </row>
     <row r="8">
@@ -702,22 +702,22 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>3600</v>
+        <v>1600</v>
       </c>
       <c r="G8" t="n">
-        <v>78700</v>
+        <v>157006</v>
       </c>
       <c r="H8" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I8" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>-4941</v>
+        <v>-11808</v>
       </c>
     </row>
     <row r="9">
@@ -733,22 +733,22 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>3700</v>
+        <v>1700</v>
       </c>
       <c r="G9" t="n">
-        <v>76908</v>
+        <v>151028</v>
       </c>
       <c r="H9" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I9" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>-5368</v>
+        <v>-11808</v>
       </c>
     </row>
     <row r="10">
@@ -764,22 +764,22 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>3800</v>
+        <v>1800</v>
       </c>
       <c r="G10" t="n">
-        <v>75690</v>
+        <v>145576</v>
       </c>
       <c r="H10" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I10" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>-5368</v>
+        <v>-10735</v>
       </c>
     </row>
     <row r="11">
@@ -795,22 +795,22 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>3900</v>
+        <v>1900</v>
       </c>
       <c r="G11" t="n">
-        <v>73944</v>
+        <v>134162</v>
       </c>
       <c r="H11" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I11" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>-5368</v>
+        <v>-9235</v>
       </c>
     </row>
     <row r="12">
@@ -826,22 +826,22 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="G12" t="n">
-        <v>72438</v>
+        <v>131346</v>
       </c>
       <c r="H12" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="I12" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>-5368</v>
+        <v>-9662</v>
       </c>
     </row>
     <row r="13">
@@ -857,22 +857,22 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>4100</v>
+        <v>2100</v>
       </c>
       <c r="G13" t="n">
-        <v>71352</v>
+        <v>126124</v>
       </c>
       <c r="H13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>-5368</v>
+        <v>-9662</v>
       </c>
     </row>
     <row r="14">
@@ -888,22 +888,22 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>4200</v>
+        <v>2200</v>
       </c>
       <c r="G14" t="n">
-        <v>68366</v>
+        <v>120712</v>
       </c>
       <c r="H14" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I14" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>-5368</v>
+        <v>-9662</v>
       </c>
     </row>
     <row r="15">
@@ -919,22 +919,22 @@
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>4300</v>
+        <v>2300</v>
       </c>
       <c r="G15" t="n">
-        <v>66983</v>
+        <v>115914</v>
       </c>
       <c r="H15" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I15" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>-5368</v>
+        <v>-8588</v>
       </c>
     </row>
     <row r="16">
@@ -950,22 +950,22 @@
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>4400</v>
+        <v>2400</v>
       </c>
       <c r="G16" t="n">
-        <v>66771</v>
+        <v>112366</v>
       </c>
       <c r="H16" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I16" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>-5368</v>
+        <v>-8588</v>
       </c>
     </row>
     <row r="17">
@@ -981,22 +981,22 @@
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>4500</v>
+        <v>2500</v>
       </c>
       <c r="G17" t="n">
-        <v>66000</v>
+        <v>107690</v>
       </c>
       <c r="H17" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I17" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>-5368</v>
+        <v>-8588</v>
       </c>
     </row>
     <row r="18">
@@ -1012,22 +1012,22 @@
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>4600</v>
+        <v>2600</v>
       </c>
       <c r="G18" t="n">
-        <v>64402</v>
+        <v>103545</v>
       </c>
       <c r="H18" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I18" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>-4294</v>
+        <v>-7514</v>
       </c>
     </row>
     <row r="19">
@@ -1043,22 +1043,22 @@
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>4700</v>
+        <v>2700</v>
       </c>
       <c r="G19" t="n">
-        <v>63266</v>
+        <v>101296</v>
       </c>
       <c r="H19" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I19" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>-4294</v>
+        <v>-7514</v>
       </c>
     </row>
     <row r="20">
@@ -1074,22 +1074,22 @@
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>4800</v>
+        <v>2800</v>
       </c>
       <c r="G20" t="n">
-        <v>62774</v>
+        <v>97749</v>
       </c>
       <c r="H20" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I20" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>-4294</v>
+        <v>-7514</v>
       </c>
     </row>
     <row r="21">
@@ -1105,22 +1105,22 @@
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>4900</v>
+        <v>2900</v>
       </c>
       <c r="G21" t="n">
-        <v>61583</v>
+        <v>95012</v>
       </c>
       <c r="H21" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I21" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>-4294</v>
+        <v>-7514</v>
       </c>
     </row>
     <row r="22">
@@ -1136,21 +1136,641 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
+        <v>3000</v>
+      </c>
+      <c r="G22" t="n">
+        <v>88776</v>
+      </c>
+      <c r="H22" t="n">
+        <v>7</v>
+      </c>
+      <c r="I22" t="n">
+        <v>7</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-6441</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="b">
+        <v>0</v>
+      </c>
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>3100</v>
+      </c>
+      <c r="G23" t="n">
+        <v>86796</v>
+      </c>
+      <c r="H23" t="n">
+        <v>7</v>
+      </c>
+      <c r="I23" t="n">
+        <v>7</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-6441</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>3200</v>
+      </c>
+      <c r="G24" t="n">
+        <v>84652</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7</v>
+      </c>
+      <c r="I24" t="n">
+        <v>7</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-6441</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>3300</v>
+      </c>
+      <c r="G25" t="n">
+        <v>84538</v>
+      </c>
+      <c r="H25" t="n">
+        <v>7</v>
+      </c>
+      <c r="I25" t="n">
+        <v>7</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>-6441</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="b">
+        <v>0</v>
+      </c>
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>3400</v>
+      </c>
+      <c r="G26" t="n">
+        <v>80956</v>
+      </c>
+      <c r="H26" t="n">
+        <v>6</v>
+      </c>
+      <c r="I26" t="n">
+        <v>6</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-6441</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="b">
+        <v>0</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="n">
+        <v>3500</v>
+      </c>
+      <c r="G27" t="n">
+        <v>79974</v>
+      </c>
+      <c r="H27" t="n">
+        <v>6</v>
+      </c>
+      <c r="I27" t="n">
+        <v>6</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-6441</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="b">
+        <v>0</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>3600</v>
+      </c>
+      <c r="G28" t="n">
+        <v>78700</v>
+      </c>
+      <c r="H28" t="n">
+        <v>6</v>
+      </c>
+      <c r="I28" t="n">
+        <v>6</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-4941</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
+        <v>3700</v>
+      </c>
+      <c r="G29" t="n">
+        <v>76908</v>
+      </c>
+      <c r="H29" t="n">
+        <v>6</v>
+      </c>
+      <c r="I29" t="n">
+        <v>6</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="n">
+        <v>3800</v>
+      </c>
+      <c r="G30" t="n">
+        <v>75690</v>
+      </c>
+      <c r="H30" t="n">
+        <v>6</v>
+      </c>
+      <c r="I30" t="n">
+        <v>6</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="b">
+        <v>0</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>3900</v>
+      </c>
+      <c r="G31" t="n">
+        <v>73944</v>
+      </c>
+      <c r="H31" t="n">
+        <v>6</v>
+      </c>
+      <c r="I31" t="n">
+        <v>6</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="b">
+        <v>0</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G32" t="n">
+        <v>72438</v>
+      </c>
+      <c r="H32" t="n">
+        <v>6</v>
+      </c>
+      <c r="I32" t="n">
+        <v>6</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="b">
+        <v>0</v>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="n">
+        <v>4100</v>
+      </c>
+      <c r="G33" t="n">
+        <v>71352</v>
+      </c>
+      <c r="H33" t="n">
+        <v>6</v>
+      </c>
+      <c r="I33" t="n">
+        <v>6</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="b">
+        <v>0</v>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>4200</v>
+      </c>
+      <c r="G34" t="n">
+        <v>68366</v>
+      </c>
+      <c r="H34" t="n">
+        <v>5</v>
+      </c>
+      <c r="I34" t="n">
+        <v>5</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="b">
+        <v>0</v>
+      </c>
+      <c r="B35" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>4300</v>
+      </c>
+      <c r="G35" t="n">
+        <v>66983</v>
+      </c>
+      <c r="H35" t="n">
+        <v>5</v>
+      </c>
+      <c r="I35" t="n">
+        <v>5</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="b">
+        <v>0</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>4400</v>
+      </c>
+      <c r="G36" t="n">
+        <v>66771</v>
+      </c>
+      <c r="H36" t="n">
+        <v>5</v>
+      </c>
+      <c r="I36" t="n">
+        <v>5</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="b">
+        <v>0</v>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="n">
+        <v>4500</v>
+      </c>
+      <c r="G37" t="n">
+        <v>66000</v>
+      </c>
+      <c r="H37" t="n">
+        <v>5</v>
+      </c>
+      <c r="I37" t="n">
+        <v>5</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>-5368</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="b">
+        <v>0</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>4600</v>
+      </c>
+      <c r="G38" t="n">
+        <v>64402</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5</v>
+      </c>
+      <c r="I38" t="n">
+        <v>5</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>-4294</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="b">
+        <v>0</v>
+      </c>
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>4700</v>
+      </c>
+      <c r="G39" t="n">
+        <v>63266</v>
+      </c>
+      <c r="H39" t="n">
+        <v>5</v>
+      </c>
+      <c r="I39" t="n">
+        <v>5</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>-4294</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="b">
+        <v>0</v>
+      </c>
+      <c r="B40" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>4800</v>
+      </c>
+      <c r="G40" t="n">
+        <v>62774</v>
+      </c>
+      <c r="H40" t="n">
+        <v>5</v>
+      </c>
+      <c r="I40" t="n">
+        <v>5</v>
+      </c>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>-4294</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="b">
+        <v>0</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="n">
+        <v>4900</v>
+      </c>
+      <c r="G41" t="n">
+        <v>61583</v>
+      </c>
+      <c r="H41" t="n">
+        <v>5</v>
+      </c>
+      <c r="I41" t="n">
+        <v>5</v>
+      </c>
+      <c r="J41" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>-4294</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="b">
+        <v>0</v>
+      </c>
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="n">
         <v>5000</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G42" t="n">
         <v>60498</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H42" t="n">
         <v>5</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I42" t="n">
         <v>5</v>
       </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
         <v>-4294</v>
       </c>
     </row>

</xml_diff>